<commit_message>
update: capitulo 1 - tabelas frequencias
</commit_message>
<xml_diff>
--- a/dados/questionario_estudantil.xlsx
+++ b/dados/questionario_estudantil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabin\OneDrive\Área de Trabalho\nocoes_de_probabilidade_e_estatistica\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB22CECE-1B00-4AED-A134-0F61FB547118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A815A2F8-98D5-4583-8D58-4650B61C179E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{EE974EFD-1A09-4360-95FE-5D32E9813000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="25">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -469,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EAFA4B-AC4C-4929-9401-2BE9280FB343}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,6 +559,24 @@
       <c r="H2" t="s">
         <v>18</v>
       </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -569,6 +602,24 @@
       </c>
       <c r="H3" t="s">
         <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -596,6 +647,24 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4">
+        <v>15</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -622,6 +691,24 @@
       <c r="H5" t="s">
         <v>18</v>
       </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5">
+        <v>20</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -648,6 +735,24 @@
       <c r="H6" t="s">
         <v>18</v>
       </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -674,6 +779,24 @@
       <c r="H7" t="s">
         <v>18</v>
       </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -700,6 +823,24 @@
       <c r="H8" t="s">
         <v>18</v>
       </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8">
+        <v>7</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -726,6 +867,24 @@
       <c r="H9" t="s">
         <v>19</v>
       </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="N9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -752,6 +911,24 @@
       <c r="H10" t="s">
         <v>18</v>
       </c>
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10">
+        <v>12</v>
+      </c>
+      <c r="N10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -778,6 +955,24 @@
       <c r="H11" t="s">
         <v>18</v>
       </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -804,6 +999,24 @@
       <c r="H12" t="s">
         <v>19</v>
       </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12">
+        <v>8</v>
+      </c>
+      <c r="N12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -830,6 +1043,24 @@
       <c r="H13" t="s">
         <v>18</v>
       </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -856,6 +1087,24 @@
       <c r="H14" t="s">
         <v>18</v>
       </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14">
+        <v>30</v>
+      </c>
+      <c r="N14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -881,6 +1130,24 @@
       </c>
       <c r="H15" t="s">
         <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -908,8 +1175,26 @@
       <c r="H16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="N16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -934,8 +1219,26 @@
       <c r="H17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17">
+        <v>18</v>
+      </c>
+      <c r="N17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -960,8 +1263,26 @@
       <c r="H18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+      <c r="N18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -986,8 +1307,26 @@
       <c r="H19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
+      </c>
+      <c r="N19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1012,8 +1351,26 @@
       <c r="H20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1038,8 +1395,26 @@
       <c r="H21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21">
+        <v>7</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21">
+        <v>14</v>
+      </c>
+      <c r="N21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1064,8 +1439,26 @@
       <c r="H22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22">
+        <v>8</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+      <c r="N22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1090,8 +1483,26 @@
       <c r="H23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+      <c r="N23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1116,8 +1527,26 @@
       <c r="H24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24">
+        <v>10</v>
+      </c>
+      <c r="N24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1142,8 +1571,26 @@
       <c r="H25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25">
+        <v>28</v>
+      </c>
+      <c r="N25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1168,8 +1615,26 @@
       <c r="H26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26">
+        <v>8</v>
+      </c>
+      <c r="K26">
+        <v>5</v>
+      </c>
+      <c r="L26" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26">
+        <v>4</v>
+      </c>
+      <c r="N26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1194,8 +1659,26 @@
       <c r="H27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27">
+        <v>5</v>
+      </c>
+      <c r="N27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1220,8 +1703,26 @@
       <c r="H28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28">
+        <v>8</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28">
+        <v>5</v>
+      </c>
+      <c r="N28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1246,8 +1747,26 @@
       <c r="H29" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29">
+        <v>10</v>
+      </c>
+      <c r="N29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1272,8 +1791,26 @@
       <c r="H30" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M30">
+        <v>12</v>
+      </c>
+      <c r="N30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1298,8 +1835,26 @@
       <c r="H31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
+      </c>
+      <c r="N31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1324,8 +1879,26 @@
       <c r="H32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+      <c r="L32" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32">
+        <v>6</v>
+      </c>
+      <c r="N32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1350,8 +1923,26 @@
       <c r="H33" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>23</v>
+      </c>
+      <c r="M33">
+        <v>20</v>
+      </c>
+      <c r="N33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1376,8 +1967,26 @@
       <c r="H34" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34">
+        <v>14</v>
+      </c>
+      <c r="N34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1402,8 +2011,26 @@
       <c r="H35" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="L35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="N35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1428,8 +2055,26 @@
       <c r="H36" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36">
+        <v>7</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36">
+        <v>25</v>
+      </c>
+      <c r="N36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1454,8 +2099,26 @@
       <c r="H37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37">
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37">
+        <v>14</v>
+      </c>
+      <c r="N37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1480,8 +2143,26 @@
       <c r="H38" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38">
+        <v>10</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+      <c r="L38" t="s">
+        <v>21</v>
+      </c>
+      <c r="M38">
+        <v>12</v>
+      </c>
+      <c r="N38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1506,8 +2187,26 @@
       <c r="H39" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39">
+        <v>6</v>
+      </c>
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39">
+        <v>10</v>
+      </c>
+      <c r="N39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1532,8 +2231,26 @@
       <c r="H40" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40">
+        <v>5</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="L40" t="s">
+        <v>23</v>
+      </c>
+      <c r="M40">
+        <v>12</v>
+      </c>
+      <c r="N40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1558,8 +2275,26 @@
       <c r="H41" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41" t="s">
+        <v>23</v>
+      </c>
+      <c r="M41">
+        <v>2</v>
+      </c>
+      <c r="N41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1584,8 +2319,26 @@
       <c r="H42" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" t="s">
+        <v>22</v>
+      </c>
+      <c r="J42">
+        <v>5</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42">
+        <v>10</v>
+      </c>
+      <c r="N42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1610,8 +2363,26 @@
       <c r="H43" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="L43" t="s">
+        <v>23</v>
+      </c>
+      <c r="M43">
+        <v>25</v>
+      </c>
+      <c r="N43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1636,8 +2407,26 @@
       <c r="H44" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>22</v>
+      </c>
+      <c r="J44">
+        <v>7</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44" t="s">
+        <v>21</v>
+      </c>
+      <c r="M44">
+        <v>14</v>
+      </c>
+      <c r="N44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1662,8 +2451,26 @@
       <c r="H45" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45">
+        <v>5</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M45">
+        <v>8</v>
+      </c>
+      <c r="N45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1688,8 +2495,26 @@
       <c r="H46" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46">
+        <v>10</v>
+      </c>
+      <c r="N46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1714,8 +2539,26 @@
       <c r="H47" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47" t="s">
+        <v>23</v>
+      </c>
+      <c r="M47">
+        <v>8</v>
+      </c>
+      <c r="N47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1740,8 +2583,26 @@
       <c r="H48" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="L48" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48">
+        <v>3</v>
+      </c>
+      <c r="N48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1766,8 +2627,26 @@
       <c r="H49" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
+        <v>23</v>
+      </c>
+      <c r="M49">
+        <v>5</v>
+      </c>
+      <c r="N49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1792,8 +2671,26 @@
       <c r="H50" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50">
+        <v>7</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50" t="s">
+        <v>21</v>
+      </c>
+      <c r="M50">
+        <v>14</v>
+      </c>
+      <c r="N50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1817,6 +2714,24 @@
       </c>
       <c r="H51" t="s">
         <v>18</v>
+      </c>
+      <c r="I51" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51">
+        <v>7</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51" t="s">
+        <v>21</v>
+      </c>
+      <c r="M51">
+        <v>20</v>
+      </c>
+      <c r="N51" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>